<commit_message>
Updating RTM & GDD-Review sheet
Signed-off-by: NorhanNassar <norhan.nassar96@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specification/Architecture/GDD/GDD_Review.xlsx
+++ b/Software Specification/Architecture/GDD/GDD_Review.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Abdelrahman\pp\Software Specification\Architecture\GDD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti data\software engineering\Folder_Structure\Software Specification\Architecture\GDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="0" windowWidth="20775" windowHeight="11040" activeTab="1"/>
+    <workbookView xWindow="4536" yWindow="0" windowWidth="20772" windowHeight="11040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>Entry Date</t>
   </si>
@@ -114,9 +114,6 @@
     <t>V1.0</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>M.Nader</t>
   </si>
   <si>
@@ -130,12 +127,21 @@
   </si>
   <si>
     <t>Requirements: Shall add the covered requirement from the SRS and add inputs and outputs from the context diagram</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Modified</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -219,7 +225,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -318,28 +324,204 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thick">
+        <color theme="3"/>
+      </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="3"/>
+      </right>
+      <top style="thick">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thick">
+        <color theme="3"/>
+      </right>
+      <top style="thick">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
       </right>
       <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thick">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thick">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="dashed">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="dashed">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -349,180 +531,45 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="1" tint="0.499984740745262"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="dashed">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="3"/>
-      </left>
-      <right style="thin">
-        <color theme="3"/>
-      </right>
-      <top style="thick">
-        <color theme="3"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="dashed">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="dashed">
+        <color theme="1" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="3"/>
-      </left>
-      <right style="thin">
-        <color theme="3"/>
-      </right>
-      <top style="thick">
-        <color theme="3"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3"/>
+        <color theme="1" tint="0.499984740745262"/>
       </left>
       <right style="thick">
-        <color theme="3"/>
-      </right>
-      <top style="thick">
-        <color theme="3"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="3"/>
-      </left>
-      <right style="thin">
-        <color theme="3"/>
-      </right>
-      <top style="thin">
-        <color theme="3"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3"/>
-      </left>
-      <right style="thin">
-        <color theme="3"/>
-      </right>
-      <top style="thin">
-        <color theme="3"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3"/>
-      </left>
-      <right style="thick">
-        <color theme="3"/>
-      </right>
-      <top style="thin">
-        <color theme="3"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="3"/>
-      </left>
-      <right style="thin">
-        <color theme="3"/>
-      </right>
-      <top style="thin">
-        <color theme="3"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="dashed">
+        <color theme="1" tint="0.499984740745262"/>
       </top>
       <bottom style="thick">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3"/>
-      </left>
-      <right style="thin">
-        <color theme="3"/>
-      </right>
-      <top style="thin">
-        <color theme="3"/>
-      </top>
-      <bottom style="thick">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3"/>
-      </left>
-      <right style="thick">
-        <color theme="3"/>
-      </right>
-      <top style="thin">
-        <color theme="3"/>
-      </top>
-      <bottom style="thick">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1" tint="0.499984740745262"/>
-      </left>
-      <right style="thin">
-        <color theme="1" tint="0.499984740745262"/>
-      </right>
-      <top style="dashed">
-        <color theme="1" tint="0.499984740745262"/>
-      </top>
-      <bottom style="dashed">
         <color theme="1" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -533,7 +580,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -553,93 +600,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -648,7 +723,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="10">
     <dxf>
       <font>
         <b/>
@@ -658,66 +733,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="5" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1111,111 +1126,111 @@
       <selection activeCell="C14" sqref="C14:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="3:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="28" t="s">
+    <row r="6" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="3:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29" t="s">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="32"/>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="33"/>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="30"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="33"/>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="24" t="s">
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="28"/>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="29"/>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="29"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C10" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="19" t="s">
+      <c r="D10" s="27"/>
+      <c r="E10" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="20"/>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="24" t="s">
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="32"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C11" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="19" t="s">
+      <c r="D11" s="33"/>
+      <c r="E11" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="20"/>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="24" t="s">
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="32"/>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C12" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="19" t="s">
+      <c r="D12" s="33"/>
+      <c r="E12" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="20"/>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="24" t="s">
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="32"/>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C13" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="21" t="s">
+      <c r="D13" s="33"/>
+      <c r="E13" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="20"/>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="26"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="20"/>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="27" t="s">
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="32"/>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C14" s="35"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="32"/>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C15" s="21" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="22"/>
@@ -1225,8 +1240,8 @@
       <c r="H15" s="22"/>
       <c r="I15" s="23"/>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="13" t="s">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C16" s="11" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="22" t="s">
@@ -1242,71 +1257,92 @@
       </c>
       <c r="I16" s="23"/>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="16">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C17" s="14">
         <v>0.1</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19" t="s">
+      <c r="E17" s="31"/>
+      <c r="F17" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19" t="s">
+      <c r="G17" s="31"/>
+      <c r="H17" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="20"/>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="14"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="20"/>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="14"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="20"/>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="14"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="20"/>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="14"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="20"/>
-    </row>
-    <row r="22" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="15"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="18"/>
-    </row>
-    <row r="23" spans="3:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="I17" s="32"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C18" s="12"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="32"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C19" s="12"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="32"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C20" s="12"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="32"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C21" s="12"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="32"/>
+    </row>
+    <row r="22" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="13"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="37"/>
+    </row>
+    <row r="23" spans="3:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
     <mergeCell ref="C15:I15"/>
     <mergeCell ref="C7:E9"/>
     <mergeCell ref="F7:I9"/>
@@ -1319,27 +1355,6 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:I13"/>
     <mergeCell ref="C14:I14"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1350,23 +1365,25 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
     <col min="6" max="6" width="60" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="25.88671875" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" customWidth="1"/>
     <col min="14" max="14" width="39" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1391,35 +1408,35 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="O1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="50" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1428,31 +1445,35 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="37">
+      <c r="I2" s="16">
         <v>43833</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="39" t="s">
+      <c r="N2" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="41"/>
+      <c r="O2" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="P2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="41"/>
-    </row>
-    <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1461,31 +1482,35 @@
       <c r="F3" s="8"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="37">
+      <c r="I3" s="16">
         <v>43833</v>
       </c>
-      <c r="J3" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="38" t="s">
+      <c r="J3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="37" t="s">
+      <c r="L3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="39" t="s">
+      <c r="M3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="40" t="s">
+      <c r="O3" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="41"/>
       <c r="P3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="41"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1494,17 +1519,17 @@
       <c r="F4" s="8"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="43"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="51"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1513,17 +1538,17 @@
       <c r="F5" s="8"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="43"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="52"/>
+    </row>
+    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1532,17 +1557,17 @@
       <c r="F6" s="8"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="43"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="53"/>
+    </row>
+    <row r="7" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1550,10 +1575,10 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H7" s="41"/>
+      <c r="I7" s="43"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1561,8 +1586,8 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="9"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="43"/>
       <c r="K8" t="s">
         <v>9</v>
       </c>
@@ -1570,7 +1595,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1578,8 +1603,8 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="9"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="43"/>
       <c r="K9" t="s">
         <v>11</v>
       </c>
@@ -1587,7 +1612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1595,10 +1620,10 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H10" s="41"/>
+      <c r="I10" s="43"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1606,10 +1631,10 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H11" s="41"/>
+      <c r="I11" s="43"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1617,10 +1642,10 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H12" s="41"/>
+      <c r="I12" s="43"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1628,10 +1653,10 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H13" s="41"/>
+      <c r="I13" s="43"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1639,10 +1664,10 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H14" s="41"/>
+      <c r="I14" s="43"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1650,10 +1675,10 @@
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H15" s="41"/>
+      <c r="I15" s="43"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1661,10 +1686,10 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="41"/>
+      <c r="I16" s="43"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1672,10 +1697,10 @@
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="41"/>
+      <c r="I17" s="43"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -1683,10 +1708,10 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="41"/>
+      <c r="I18" s="43"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -1694,10 +1719,10 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="41"/>
+      <c r="I19" s="43"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1705,10 +1730,10 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="41"/>
+      <c r="I20" s="43"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1716,10 +1741,10 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H21" s="41"/>
+      <c r="I21" s="43"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1727,10 +1752,10 @@
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="41"/>
+      <c r="I22" s="43"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1738,10 +1763,10 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="41"/>
+      <c r="I23" s="43"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1749,10 +1774,10 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H24" s="41"/>
+      <c r="I24" s="43"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1760,10 +1785,10 @@
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H25" s="41"/>
+      <c r="I25" s="43"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1771,10 +1796,10 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26" s="41"/>
+      <c r="I26" s="43"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1782,10 +1807,10 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H27" s="41"/>
+      <c r="I27" s="43"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1793,10 +1818,10 @@
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H28" s="41"/>
+      <c r="I28" s="43"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1804,10 +1829,10 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="9"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H29" s="41"/>
+      <c r="I29" s="43"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -1815,10 +1840,10 @@
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30" s="41"/>
+      <c r="I30" s="43"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1826,74 +1851,68 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="12"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="43"/>
+    </row>
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="43"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="14" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="equal">
       <formula>$G$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" stopIfTrue="1" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="10" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1">
-    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="equal">
       <formula>$G$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1">
-    <cfRule type="cellIs" dxfId="1" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G32 H2:H32">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:H32">
       <formula1>$F$34:$F$35</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1">
-      <formula1>$F$34:$F$35</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1:O3 O5:O6">
+      <formula1>$T$16:$T$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3">
-      <formula1>$K$3:$K$4</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1 P4:P6">
-      <formula1>$K$5:$K$6</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1 O4:O6">
-      <formula1>$K$3:$K$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P3 P5:P6">
+      <formula1>$Q$18:$Q$19</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>